<commit_message>
- Se agregó el testing de lo que había hecho Testing Sprint #3.xlsx
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/Agiles/SPRINT 3/Testing Sprint #3.xlsx
+++ b/Documentacion/Testing/Agiles/SPRINT 3/Testing Sprint #3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="51">
   <si>
     <t>QUE GOLAZO!</t>
   </si>
@@ -166,6 +166,69 @@
   </si>
   <si>
     <t xml:space="preserve">No se visualiza la opción "Ver Fixture" </t>
+  </si>
+  <si>
+    <t>No se visualiza la opción "Cargar Resultados"</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>Se cargaron los resultados de la fecha completa</t>
+  </si>
+  <si>
+    <t>Errores Cosméticos</t>
+  </si>
+  <si>
+    <t>- Una vez que toqué el botón guardar, debería mostrarme solos los txt llenos de los partidos válidos, es decir los de la fecha libre NO. Si bien en la Base de datos no lo guarda, si quedan en los txt el estado de los txt</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>Formato incorrecto</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>Error en la consulta sql</t>
+  </si>
+  <si>
+    <t>Falló</t>
+  </si>
+  <si>
+    <t>No valida que se ingresen numeros negativos</t>
+  </si>
+  <si>
+    <t>Pendiente de Corrección</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>Formato inválido</t>
+  </si>
+  <si>
+    <t>TC_008</t>
+  </si>
+  <si>
+    <t>No me tira error</t>
+  </si>
+  <si>
+    <t>No valida que uno de los txt esté vacío</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Bloqueado</t>
+  </si>
+  <si>
+    <t>No me muestra el botón Cancelar</t>
   </si>
 </sst>
 </file>
@@ -201,7 +264,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +280,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -265,17 +334,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,43 +675,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -676,35 +746,47 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>41790</v>
       </c>
       <c r="I5" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="H6" s="9">
+        <v>41791</v>
+      </c>
+      <c r="I6" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -783,7 +865,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,43 +879,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -864,39 +946,51 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>41790</v>
       </c>
       <c r="I5" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="H6" s="9">
+        <v>41791</v>
+      </c>
+      <c r="I6" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -935,56 +1029,57 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="A1:I8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="40.140625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1015,23 +1110,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="9">
+        <v>41791</v>
+      </c>
+      <c r="I5" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1042,9 +1145,7 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1077,59 +1178,60 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="40.140625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1160,16 +1262,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="9">
+        <v>41791</v>
+      </c>
+      <c r="I5" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1203,6 +1317,16 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1219,7 +1343,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,43 +1356,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1300,15 +1424,27 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="9">
+        <v>41791</v>
+      </c>
+      <c r="I5" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1358,7 +1494,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,43 +1507,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1438,16 +1574,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="F5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="9">
+        <v>41791</v>
+      </c>
+      <c r="I5" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1497,7 +1649,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,43 +1662,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1578,15 +1730,27 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="9">
+        <v>41791</v>
+      </c>
+      <c r="I5" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1636,7 +1800,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A5:A8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,43 +1813,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1716,16 +1880,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="F5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="9">
+        <v>41791</v>
+      </c>
+      <c r="I5" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1774,8 +1954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,43 +1968,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1855,16 +2035,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="G5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="9">
+        <v>41791</v>
+      </c>
+      <c r="I5" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>

</xml_diff>